<commit_message>
fix the content of `parse2jsonCover`.
</commit_message>
<xml_diff>
--- a/test/assets/excel.xlsx
+++ b/test/assets/excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11120"/>
+    <workbookView windowWidth="28800" windowHeight="11720"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
   <si>
     <t>filename</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test1 key</t>
     </r>
     <r>
@@ -241,6 +247,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test1 key</t>
     </r>
     <r>
@@ -261,6 +273,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test1 key2</t>
     </r>
     <r>
@@ -281,6 +299,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test2 key</t>
     </r>
     <r>
@@ -298,6 +322,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test2 key</t>
     </r>
     <r>
@@ -318,6 +348,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test2 key2</t>
     </r>
     <r>
@@ -334,10 +370,36 @@
     <t>test2 key2 value</t>
   </si>
   <si>
+    <t>for test2[1].key2</t>
+  </si>
+  <si>
+    <r>
+      <t>test2 key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="华文宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>值，覆盖</t>
+    </r>
+  </si>
+  <si>
+    <t>test2 key value, cover</t>
+  </si>
+  <si>
     <t>fortest3.key</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">test3 </t>
     </r>
     <r>
@@ -358,6 +420,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">test3 </t>
     </r>
     <r>
@@ -378,6 +446,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">test4 </t>
     </r>
     <r>
@@ -398,6 +472,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">test4 </t>
     </r>
     <r>
@@ -482,9 +562,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -546,8 +626,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,8 +710,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -570,15 +734,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,83 +750,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -703,19 +783,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -727,7 +795,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,13 +819,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,55 +831,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,25 +855,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,7 +897,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -865,19 +915,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,26 +1009,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -969,6 +1034,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -979,6 +1059,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -998,22 +1093,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1022,142 +1102,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1538,10 +1618,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:Z196"/>
+  <dimension ref="A1:Z197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80357142857143" defaultRowHeight="17.6"/>
@@ -2357,9 +2437,15 @@
       <c r="Z24" s="6"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="A25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>63</v>
+      </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -7172,6 +7258,11 @@
       <c r="Y196" s="6"/>
       <c r="Z196" s="6"/>
     </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A7:A9"/>
@@ -7187,7 +7278,7 @@
   <dimension ref="A1:Z200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80357142857143" defaultRowHeight="17.6"/>
@@ -7200,13 +7291,13 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -7234,7 +7325,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -7264,13 +7355,13 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -12838,10 +12929,10 @@
         <v>200</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -12872,10 +12963,10 @@
         <v>404</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -18460,7 +18551,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -18472,49 +18563,49 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>76</v>
+      <c r="B3" s="2" t="s">
+        <v>81</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1"/>
     </row>

</xml_diff>

<commit_message>
Feature: Parsing entries can be specified.
</commit_message>
<xml_diff>
--- a/test/assets/excel.xlsx
+++ b/test/assets/excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11720"/>
+    <workbookView windowWidth="28800" windowHeight="11820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
   <si>
     <t>filename</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>test2 key</t>
     </r>
     <r>
@@ -515,6 +521,12 @@
     <t>Internet</t>
   </si>
   <si>
+    <t>首行无key</t>
+  </si>
+  <si>
+    <t>no key</t>
+  </si>
+  <si>
     <t>成功</t>
   </si>
   <si>
@@ -562,10 +574,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -626,8 +638,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -636,7 +663,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -649,15 +676,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -672,24 +693,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -702,11 +707,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -726,7 +738,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -734,7 +746,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -748,9 +760,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -783,7 +795,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,7 +891,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -807,7 +939,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,145 +963,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1013,7 +1025,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1033,6 +1075,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1048,36 +1099,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1088,156 +1109,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1620,8 +1632,8 @@
   <sheetPr/>
   <dimension ref="A1:Z197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80357142857143" defaultRowHeight="17.6"/>
@@ -12912,10 +12924,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:Z200"/>
+  <dimension ref="A1:Z201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80357142857143" defaultRowHeight="17.6"/>
@@ -12924,48 +12936,22 @@
     <col min="2" max="26" width="12.8928571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" s="3">
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="3">
         <v>200</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" s="7">
-        <v>404</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D2" s="6"/>
@@ -12993,9 +12979,15 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="7">
+        <v>404</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -13049,9 +13041,9 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -13077,9 +13069,9 @@
       <c r="Z5" s="6"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -13218,7 +13210,7 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -13245,7 +13237,7 @@
       <c r="Z11" s="6"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="6"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="6"/>
@@ -13301,8 +13293,8 @@
       <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -13329,7 +13321,7 @@
       <c r="Z14" s="6"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="6"/>
@@ -13441,9 +13433,9 @@
       <c r="Z18" s="6"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -18536,9 +18528,37 @@
       <c r="Y200" s="6"/>
       <c r="Z200" s="6"/>
     </row>
+    <row r="201" spans="1:26">
+      <c r="A201" s="6"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+      <c r="D201" s="6"/>
+      <c r="E201" s="6"/>
+      <c r="F201" s="6"/>
+      <c r="G201" s="6"/>
+      <c r="H201" s="6"/>
+      <c r="I201" s="6"/>
+      <c r="J201" s="6"/>
+      <c r="K201" s="6"/>
+      <c r="L201" s="6"/>
+      <c r="M201" s="6"/>
+      <c r="N201" s="6"/>
+      <c r="O201" s="6"/>
+      <c r="P201" s="6"/>
+      <c r="Q201" s="6"/>
+      <c r="R201" s="6"/>
+      <c r="S201" s="6"/>
+      <c r="T201" s="6"/>
+      <c r="U201" s="6"/>
+      <c r="V201" s="6"/>
+      <c r="W201" s="6"/>
+      <c r="X201" s="6"/>
+      <c r="Y201" s="6"/>
+      <c r="Z201" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -18563,49 +18583,49 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>78</v>
+      <c r="B3" s="2" t="s">
+        <v>83</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>79</v>
+      <c r="C3" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1"/>
     </row>

</xml_diff>